<commit_message>
Fresh update for playtesting
</commit_message>
<xml_diff>
--- a/data/CommonEvents.xlsx
+++ b/data/CommonEvents.xlsx
@@ -19770,8 +19770,8 @@
 約束だよ。</t>
   </si>
   <si>
-    <t>\n&lt;ロメリア&gt;Alsy... You must never...
-ever ever die out on me okay? Promise me.</t>
+    <t>\n&lt;ロメリア&gt;あにき、絶対・・・
+絶対死んじゃったりしないでね。約束だよ。</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;まさか淫魔なんかにえっちなことされて
@@ -19779,8 +19779,8 @@
 なんかちょっと、気が緩んだ顔してる・・・</t>
   </si>
   <si>
-    <t>\n&lt;ロメリア&gt;You're not enjoying those succubus doing lewd things
-to you right? You somehow look more relaxed than usual...</t>
+    <t>\n&lt;ロメリア&gt;まさか淫魔なんかにえっちなことされて
+喜んだりしてないよね？なんかちょっと、気が緩んだ顔してる・・・</t>
   </si>
   <si>
     <t>\n&lt;ロメリア&gt;肌寒い気がするのに

</xml_diff>